<commit_message>
December 2021 - Release
Minor updates across a few diagrams, and a number of new diagrams (Windows 365, Defender for Business, and Microsoft Visio).
Two large updates to m365maps.com: Draw on Diagrams and add Text to Diagrams..
Please see the change log and user guide on m365maps.com for more information.
</commit_message>
<xml_diff>
--- a/Microsoft 365 License Matrix.xlsx
+++ b/Microsoft 365 License Matrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="798" documentId="13_ncr:40009_{1420BF28-4C29-4990-B2CC-D0D9EF7DD0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57086A8D-B150-44AF-A85B-1D506610AA7B}"/>
+  <xr:revisionPtr revIDLastSave="882" documentId="13_ncr:40009_{1420BF28-4C29-4990-B2CC-D0D9EF7DD0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F35B42F-06F7-4797-A3AC-63EBBC7BE77C}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15400" yWindow="6450" windowWidth="18240" windowHeight="11780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="397">
   <si>
     <t>Enterprise Mobility + Security</t>
   </si>
@@ -1157,9 +1157,6 @@
     <t>50 GB</t>
   </si>
   <si>
-    <t>Unlimited</t>
-  </si>
-  <si>
     <t>F5 Sec + Comp</t>
   </si>
   <si>
@@ -1227,6 +1224,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>1.5 TB</t>
   </si>
 </sst>
 </file>
@@ -2757,41 +2757,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.23046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.23046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9.3828125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="171.69140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="171.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="28">
-        <v>44474</v>
+        <v>44553</v>
       </c>
       <c r="B1" s="66" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C1" s="67"/>
       <c r="D1" s="68"/>
@@ -2822,18 +2822,18 @@
       <c r="U1" s="67"/>
       <c r="V1" s="68"/>
     </row>
-    <row r="2" spans="1:23" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>278</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>380</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>381</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="23" t="s">
         <v>382</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>383</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>283</v>
@@ -2857,7 +2857,7 @@
         <v>289</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>290</v>
@@ -2872,10 +2872,10 @@
         <v>293</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="R2" s="33" t="s">
         <v>385</v>
-      </c>
-      <c r="R2" s="33" t="s">
-        <v>386</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>295</v>
@@ -2893,7 +2893,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="36" t="s">
         <v>299</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>294</v>
       </c>
       <c r="R3" s="35" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S3" s="35" t="s">
         <v>295</v>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="W3" s="38"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>127</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>194</v>
       </c>
@@ -3014,7 +3014,7 @@
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
       <c r="L5" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M5" s="7" t="s">
         <v>359</v>
@@ -3042,41 +3042,41 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>114</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>359</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N6" s="14"/>
       <c r="O6" s="14"/>
@@ -3095,7 +3095,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>354</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>355</v>
       </c>
@@ -3169,7 +3169,7 @@
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
       <c r="L8" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M8" s="7" t="s">
         <v>359</v>
@@ -3197,7 +3197,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>272</v>
       </c>
@@ -3228,7 +3228,7 @@
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M9" s="7" t="s">
         <v>359</v>
@@ -3256,7 +3256,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>368</v>
       </c>
@@ -3287,7 +3287,7 @@
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
       <c r="L10" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M10" s="7" t="s">
         <v>359</v>
@@ -3315,7 +3315,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
@@ -3342,7 +3342,7 @@
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
       <c r="L11" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M11" s="7" t="s">
         <v>359</v>
@@ -3366,7 +3366,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>138</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>120</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>118</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>180</v>
       </c>
@@ -3565,7 +3565,7 @@
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
       <c r="L16" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M16" s="7" t="s">
         <v>359</v>
@@ -3593,7 +3593,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>174</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>353</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>358</v>
       </c>
@@ -3692,7 +3692,9 @@
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="8"/>
+      <c r="G19" s="8" t="s">
+        <v>359</v>
+      </c>
       <c r="H19" s="7"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -3728,7 +3730,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>2</v>
       </c>
@@ -3759,7 +3761,7 @@
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
       <c r="L20" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M20" s="7" t="s">
         <v>345</v>
@@ -3787,7 +3789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -3795,10 +3797,10 @@
         <v>372</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>372</v>
@@ -3807,24 +3809,24 @@
         <v>372</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
       <c r="P21" s="8" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="Q21" s="7" t="s">
         <v>372</v>
@@ -3833,18 +3835,18 @@
         <v>372</v>
       </c>
       <c r="S21" s="14" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="T21" s="14"/>
       <c r="U21" s="14"/>
       <c r="V21" s="8" t="s">
-        <v>373</v>
+        <v>396</v>
       </c>
       <c r="W21" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>183</v>
       </c>
@@ -3873,7 +3875,7 @@
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
       <c r="L22" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M22" s="7" t="s">
         <v>359</v>
@@ -3901,7 +3903,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>189</v>
       </c>
@@ -3920,7 +3922,7 @@
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
       <c r="L23" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M23" s="7" t="s">
         <v>359</v>
@@ -3940,7 +3942,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>129</v>
       </c>
@@ -3983,7 +3985,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>146</v>
       </c>
@@ -4026,7 +4028,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>186</v>
       </c>
@@ -4044,7 +4046,7 @@
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="14" t="s">
@@ -4079,7 +4081,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>313</v>
       </c>
@@ -4102,7 +4104,7 @@
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
       <c r="L27" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M27" s="7" t="s">
         <v>359</v>
@@ -4130,7 +4132,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>360</v>
       </c>
@@ -4151,7 +4153,7 @@
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
       <c r="L28" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M28" s="7" t="s">
         <v>359</v>
@@ -4175,7 +4177,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>305</v>
       </c>
@@ -4198,7 +4200,7 @@
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
       <c r="L29" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M29" s="12" t="s">
         <v>303</v>
@@ -4224,7 +4226,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
@@ -4253,7 +4255,7 @@
       <c r="J30" s="14"/>
       <c r="K30" s="14"/>
       <c r="L30" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M30" s="7" t="s">
         <v>359</v>
@@ -4277,7 +4279,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>131</v>
       </c>
@@ -4320,7 +4322,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
         <v>135</v>
       </c>
@@ -4363,7 +4365,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
         <v>148</v>
       </c>
@@ -4406,7 +4408,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
         <v>170</v>
       </c>
@@ -4449,7 +4451,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
         <v>168</v>
       </c>
@@ -4492,7 +4494,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
         <v>144</v>
       </c>
@@ -4535,7 +4537,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
         <v>133</v>
       </c>
@@ -4578,7 +4580,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38" s="18" t="s">
         <v>276</v>
       </c>
@@ -4623,7 +4625,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39" s="19" t="s">
         <v>161</v>
       </c>
@@ -4668,7 +4670,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40" s="19" t="s">
         <v>249</v>
       </c>
@@ -4713,7 +4715,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41" s="19" t="s">
         <v>159</v>
       </c>
@@ -4758,7 +4760,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" s="19" t="s">
         <v>157</v>
       </c>
@@ -4803,7 +4805,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>20</v>
       </c>
@@ -4826,7 +4828,7 @@
         <v>359</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I43" s="14" t="s">
         <v>359</v>
@@ -4834,7 +4836,7 @@
       <c r="J43" s="14"/>
       <c r="K43" s="14"/>
       <c r="L43" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M43" s="7" t="s">
         <v>359</v>
@@ -4862,7 +4864,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>33</v>
       </c>
@@ -4889,7 +4891,7 @@
       <c r="J44" s="14"/>
       <c r="K44" s="14"/>
       <c r="L44" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M44" s="7" t="s">
         <v>359</v>
@@ -4917,7 +4919,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>12</v>
       </c>
@@ -4948,7 +4950,7 @@
       <c r="J45" s="14"/>
       <c r="K45" s="14"/>
       <c r="L45" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M45" s="7" t="s">
         <v>359</v>
@@ -4976,7 +4978,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>37</v>
       </c>
@@ -5005,7 +5007,7 @@
       <c r="J46" s="14"/>
       <c r="K46" s="14"/>
       <c r="L46" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M46" s="7" t="s">
         <v>359</v>
@@ -5033,7 +5035,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>35</v>
       </c>
@@ -5062,7 +5064,7 @@
       <c r="J47" s="14"/>
       <c r="K47" s="14"/>
       <c r="L47" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M47" s="7" t="s">
         <v>359</v>
@@ -5090,7 +5092,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>15</v>
       </c>
@@ -5117,7 +5119,7 @@
       <c r="J48" s="14"/>
       <c r="K48" s="14"/>
       <c r="L48" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M48" s="12" t="s">
         <v>332</v>
@@ -5141,7 +5143,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>142</v>
       </c>
@@ -5158,7 +5160,7 @@
       <c r="J49" s="14"/>
       <c r="K49" s="14"/>
       <c r="L49" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M49" s="7"/>
       <c r="N49" s="14"/>
@@ -5180,7 +5182,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>314</v>
       </c>
@@ -5211,7 +5213,7 @@
       <c r="J50" s="14"/>
       <c r="K50" s="14"/>
       <c r="L50" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M50" s="7" t="s">
         <v>359</v>
@@ -5232,12 +5234,14 @@
       </c>
       <c r="T50" s="14"/>
       <c r="U50" s="14"/>
-      <c r="V50" s="8"/>
+      <c r="V50" s="8" t="s">
+        <v>359</v>
+      </c>
       <c r="W50" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>30</v>
       </c>
@@ -5268,7 +5272,7 @@
       <c r="J51" s="14"/>
       <c r="K51" s="14"/>
       <c r="L51" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M51" s="7" t="s">
         <v>359</v>
@@ -5289,12 +5293,14 @@
       </c>
       <c r="T51" s="14"/>
       <c r="U51" s="14"/>
-      <c r="V51" s="8"/>
+      <c r="V51" s="8" t="s">
+        <v>359</v>
+      </c>
       <c r="W51" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>6</v>
       </c>
@@ -5316,14 +5322,16 @@
       <c r="G52" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="H52" s="7"/>
+      <c r="H52" s="7" t="s">
+        <v>344</v>
+      </c>
       <c r="I52" s="14" t="s">
         <v>344</v>
       </c>
       <c r="J52" s="14"/>
       <c r="K52" s="14"/>
       <c r="L52" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M52" s="7" t="s">
         <v>365</v>
@@ -5351,7 +5359,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>269</v>
       </c>
@@ -5366,7 +5374,7 @@
       <c r="J53" s="14"/>
       <c r="K53" s="14"/>
       <c r="L53" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M53" s="7"/>
       <c r="N53" s="14"/>
@@ -5390,7 +5398,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>112</v>
       </c>
@@ -5407,7 +5415,7 @@
       <c r="J54" s="14"/>
       <c r="K54" s="14"/>
       <c r="L54" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M54" s="7"/>
       <c r="N54" s="14"/>
@@ -5427,7 +5435,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>10</v>
       </c>
@@ -5458,7 +5466,7 @@
       <c r="J55" s="14"/>
       <c r="K55" s="14"/>
       <c r="L55" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M55" s="7" t="s">
         <v>359</v>
@@ -5486,7 +5494,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>328</v>
       </c>
@@ -5515,7 +5523,7 @@
       <c r="J56" s="14"/>
       <c r="K56" s="14"/>
       <c r="L56" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M56" s="7" t="s">
         <v>359</v>
@@ -5543,7 +5551,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>329</v>
       </c>
@@ -5572,7 +5580,7 @@
       <c r="J57" s="14"/>
       <c r="K57" s="14"/>
       <c r="L57" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M57" s="7" t="s">
         <v>359</v>
@@ -5600,7 +5608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>116</v>
       </c>
@@ -5617,7 +5625,7 @@
       <c r="J58" s="14"/>
       <c r="K58" s="14"/>
       <c r="L58" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M58" s="7"/>
       <c r="N58" s="14"/>
@@ -5637,7 +5645,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>39</v>
       </c>
@@ -5666,7 +5674,7 @@
       <c r="J59" s="14"/>
       <c r="K59" s="14"/>
       <c r="L59" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M59" s="7" t="s">
         <v>359</v>
@@ -5690,7 +5698,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>123</v>
       </c>
@@ -5733,7 +5741,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>331</v>
       </c>
@@ -5748,7 +5756,7 @@
       <c r="J61" s="14"/>
       <c r="K61" s="14"/>
       <c r="L61" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M61" s="7"/>
       <c r="N61" s="14"/>
@@ -5772,7 +5780,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>150</v>
       </c>
@@ -5815,7 +5823,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>356</v>
       </c>
@@ -5833,7 +5841,7 @@
       </c>
       <c r="H63" s="7"/>
       <c r="I63" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J63" s="14"/>
       <c r="K63" s="24" t="s">
@@ -5870,7 +5878,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>155</v>
       </c>
@@ -5913,7 +5921,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>267</v>
       </c>
@@ -5928,7 +5936,7 @@
       <c r="J65" s="14"/>
       <c r="K65" s="14"/>
       <c r="L65" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M65" s="7"/>
       <c r="N65" s="14"/>
@@ -5952,7 +5960,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>4</v>
       </c>
@@ -5983,7 +5991,7 @@
       <c r="J66" s="14"/>
       <c r="K66" s="14"/>
       <c r="L66" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M66" s="7" t="s">
         <v>311</v>
@@ -6011,7 +6019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>330</v>
       </c>
@@ -6042,7 +6050,7 @@
       <c r="J67" s="14"/>
       <c r="K67" s="14"/>
       <c r="L67" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M67" s="7" t="s">
         <v>359</v>
@@ -6070,7 +6078,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>18</v>
       </c>
@@ -6101,7 +6109,7 @@
       <c r="J68" s="14"/>
       <c r="K68" s="14"/>
       <c r="L68" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M68" s="7" t="s">
         <v>359</v>
@@ -6129,7 +6137,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>308</v>
       </c>
@@ -6170,7 +6178,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>8</v>
       </c>
@@ -6201,7 +6209,7 @@
       <c r="J70" s="14"/>
       <c r="K70" s="14"/>
       <c r="L70" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M70" s="7" t="s">
         <v>359</v>
@@ -6229,7 +6237,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A71" s="44" t="s">
         <v>0</v>
       </c>
@@ -6268,7 +6276,7 @@
       </c>
       <c r="W71" s="48"/>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>335</v>
       </c>
@@ -6287,7 +6295,7 @@
       <c r="J72" s="14"/>
       <c r="K72" s="14"/>
       <c r="L72" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M72" s="7" t="s">
         <v>359</v>
@@ -6311,7 +6319,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>317</v>
       </c>
@@ -6330,7 +6338,7 @@
       <c r="J73" s="14"/>
       <c r="K73" s="14"/>
       <c r="L73" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M73" s="7" t="s">
         <v>359</v>
@@ -6354,7 +6362,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
         <v>264</v>
       </c>
@@ -6395,7 +6403,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A75" s="17" t="s">
         <v>255</v>
       </c>
@@ -6436,7 +6444,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
         <v>256</v>
       </c>
@@ -6477,7 +6485,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A77" s="17" t="s">
         <v>258</v>
       </c>
@@ -6518,7 +6526,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A78" s="17" t="s">
         <v>262</v>
       </c>
@@ -6559,7 +6567,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A79" s="17" t="s">
         <v>260</v>
       </c>
@@ -6600,7 +6608,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A80" s="18" t="s">
         <v>86</v>
       </c>
@@ -6618,19 +6626,13 @@
       <c r="I80" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J80" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J80" s="14"/>
       <c r="K80" s="14"/>
-      <c r="L80" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L80" s="8"/>
       <c r="M80" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N80" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N80" s="14"/>
       <c r="O80" s="14"/>
       <c r="P80" s="8" t="s">
         <v>359</v>
@@ -6640,9 +6642,7 @@
       <c r="S80" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T80" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T80" s="14"/>
       <c r="U80" s="14"/>
       <c r="V80" s="8" t="s">
         <v>359</v>
@@ -6651,7 +6651,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A81" s="19" t="s">
         <v>73</v>
       </c>
@@ -6669,19 +6669,13 @@
       <c r="I81" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J81" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J81" s="14"/>
       <c r="K81" s="14"/>
-      <c r="L81" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L81" s="8"/>
       <c r="M81" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N81" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N81" s="14"/>
       <c r="O81" s="14"/>
       <c r="P81" s="8" t="s">
         <v>359</v>
@@ -6691,9 +6685,7 @@
       <c r="S81" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T81" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T81" s="14"/>
       <c r="U81" s="14"/>
       <c r="V81" s="8" t="s">
         <v>359</v>
@@ -6702,7 +6694,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A82" s="19" t="s">
         <v>76</v>
       </c>
@@ -6720,19 +6712,13 @@
       <c r="I82" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J82" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J82" s="14"/>
       <c r="K82" s="14"/>
-      <c r="L82" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L82" s="8"/>
       <c r="M82" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N82" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N82" s="14"/>
       <c r="O82" s="14"/>
       <c r="P82" s="8" t="s">
         <v>359</v>
@@ -6742,9 +6728,7 @@
       <c r="S82" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T82" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T82" s="14"/>
       <c r="U82" s="14"/>
       <c r="V82" s="8" t="s">
         <v>359</v>
@@ -6753,7 +6737,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A83" s="19" t="s">
         <v>87</v>
       </c>
@@ -6771,19 +6755,13 @@
       <c r="I83" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J83" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J83" s="14"/>
       <c r="K83" s="14"/>
-      <c r="L83" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L83" s="8"/>
       <c r="M83" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N83" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N83" s="14"/>
       <c r="O83" s="14"/>
       <c r="P83" s="8" t="s">
         <v>359</v>
@@ -6793,9 +6771,7 @@
       <c r="S83" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T83" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T83" s="14"/>
       <c r="U83" s="14"/>
       <c r="V83" s="8" t="s">
         <v>359</v>
@@ -6804,7 +6780,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A84" s="19" t="s">
         <v>93</v>
       </c>
@@ -6822,19 +6798,13 @@
       <c r="I84" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J84" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J84" s="14"/>
       <c r="K84" s="14"/>
-      <c r="L84" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L84" s="8"/>
       <c r="M84" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N84" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N84" s="14"/>
       <c r="O84" s="14"/>
       <c r="P84" s="8" t="s">
         <v>359</v>
@@ -6844,9 +6814,7 @@
       <c r="S84" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T84" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T84" s="14"/>
       <c r="U84" s="14"/>
       <c r="V84" s="8" t="s">
         <v>359</v>
@@ -6855,7 +6823,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A85" s="19" t="s">
         <v>70</v>
       </c>
@@ -6873,19 +6841,13 @@
       <c r="I85" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J85" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J85" s="14"/>
       <c r="K85" s="14"/>
-      <c r="L85" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L85" s="8"/>
       <c r="M85" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N85" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N85" s="14"/>
       <c r="O85" s="14"/>
       <c r="P85" s="8" t="s">
         <v>359</v>
@@ -6895,9 +6857,7 @@
       <c r="S85" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T85" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T85" s="14"/>
       <c r="U85" s="14"/>
       <c r="V85" s="8" t="s">
         <v>359</v>
@@ -6906,7 +6866,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A86" s="19" t="s">
         <v>323</v>
       </c>
@@ -6924,19 +6884,13 @@
       <c r="I86" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J86" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J86" s="14"/>
       <c r="K86" s="14"/>
-      <c r="L86" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L86" s="8"/>
       <c r="M86" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N86" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N86" s="14"/>
       <c r="O86" s="14"/>
       <c r="P86" s="8" t="s">
         <v>359</v>
@@ -6946,9 +6900,7 @@
       <c r="S86" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T86" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T86" s="14"/>
       <c r="U86" s="14"/>
       <c r="V86" s="8" t="s">
         <v>359</v>
@@ -6957,7 +6909,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A87" s="19" t="s">
         <v>78</v>
       </c>
@@ -6975,19 +6927,13 @@
       <c r="I87" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J87" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J87" s="14"/>
       <c r="K87" s="14"/>
-      <c r="L87" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L87" s="8"/>
       <c r="M87" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N87" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N87" s="14"/>
       <c r="O87" s="14"/>
       <c r="P87" s="8" t="s">
         <v>359</v>
@@ -6997,9 +6943,7 @@
       <c r="S87" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T87" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T87" s="14"/>
       <c r="U87" s="14"/>
       <c r="V87" s="8" t="s">
         <v>359</v>
@@ -7008,7 +6952,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A88" s="19" t="s">
         <v>84</v>
       </c>
@@ -7026,19 +6970,13 @@
       <c r="I88" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J88" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J88" s="14"/>
       <c r="K88" s="14"/>
-      <c r="L88" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L88" s="8"/>
       <c r="M88" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N88" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N88" s="14"/>
       <c r="O88" s="14"/>
       <c r="P88" s="8" t="s">
         <v>359</v>
@@ -7048,9 +6986,7 @@
       <c r="S88" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T88" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T88" s="14"/>
       <c r="U88" s="14"/>
       <c r="V88" s="8" t="s">
         <v>359</v>
@@ -7059,7 +6995,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A89" s="19" t="s">
         <v>89</v>
       </c>
@@ -7077,19 +7013,13 @@
       <c r="I89" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J89" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J89" s="14"/>
       <c r="K89" s="14"/>
-      <c r="L89" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L89" s="8"/>
       <c r="M89" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N89" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N89" s="14"/>
       <c r="O89" s="14"/>
       <c r="P89" s="8" t="s">
         <v>359</v>
@@ -7099,9 +7029,7 @@
       <c r="S89" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T89" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T89" s="14"/>
       <c r="U89" s="14"/>
       <c r="V89" s="8" t="s">
         <v>359</v>
@@ -7110,7 +7038,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A90" s="19" t="s">
         <v>95</v>
       </c>
@@ -7128,19 +7056,13 @@
       <c r="I90" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J90" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J90" s="14"/>
       <c r="K90" s="14"/>
-      <c r="L90" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L90" s="8"/>
       <c r="M90" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N90" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N90" s="14"/>
       <c r="O90" s="14"/>
       <c r="P90" s="8" t="s">
         <v>359</v>
@@ -7150,9 +7072,7 @@
       <c r="S90" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T90" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T90" s="14"/>
       <c r="U90" s="14"/>
       <c r="V90" s="8" t="s">
         <v>359</v>
@@ -7161,7 +7081,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A91" s="19" t="s">
         <v>82</v>
       </c>
@@ -7179,19 +7099,13 @@
       <c r="I91" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J91" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J91" s="14"/>
       <c r="K91" s="14"/>
-      <c r="L91" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L91" s="8"/>
       <c r="M91" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N91" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N91" s="14"/>
       <c r="O91" s="14"/>
       <c r="P91" s="8" t="s">
         <v>359</v>
@@ -7201,9 +7115,7 @@
       <c r="S91" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T91" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T91" s="14"/>
       <c r="U91" s="14"/>
       <c r="V91" s="8" t="s">
         <v>359</v>
@@ -7212,7 +7124,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A92" s="19" t="s">
         <v>307</v>
       </c>
@@ -7230,19 +7142,13 @@
       <c r="I92" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J92" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J92" s="14"/>
       <c r="K92" s="14"/>
-      <c r="L92" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L92" s="8"/>
       <c r="M92" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N92" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N92" s="14"/>
       <c r="O92" s="14"/>
       <c r="P92" s="8" t="s">
         <v>359</v>
@@ -7252,9 +7158,7 @@
       <c r="S92" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T92" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T92" s="14"/>
       <c r="U92" s="14"/>
       <c r="V92" s="8" t="s">
         <v>359</v>
@@ -7263,7 +7167,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A93" s="19" t="s">
         <v>325</v>
       </c>
@@ -7281,19 +7185,13 @@
       <c r="I93" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J93" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J93" s="14"/>
       <c r="K93" s="14"/>
-      <c r="L93" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L93" s="8"/>
       <c r="M93" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N93" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N93" s="14"/>
       <c r="O93" s="14"/>
       <c r="P93" s="8" t="s">
         <v>359</v>
@@ -7303,9 +7201,7 @@
       <c r="S93" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T93" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T93" s="14"/>
       <c r="U93" s="14"/>
       <c r="V93" s="8" t="s">
         <v>359</v>
@@ -7314,7 +7210,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A94" s="19" t="s">
         <v>324</v>
       </c>
@@ -7332,19 +7228,13 @@
       <c r="I94" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J94" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J94" s="14"/>
       <c r="K94" s="14"/>
-      <c r="L94" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L94" s="8"/>
       <c r="M94" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N94" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N94" s="14"/>
       <c r="O94" s="14"/>
       <c r="P94" s="8" t="s">
         <v>359</v>
@@ -7354,9 +7244,7 @@
       <c r="S94" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T94" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T94" s="14"/>
       <c r="U94" s="14"/>
       <c r="V94" s="8" t="s">
         <v>359</v>
@@ -7365,7 +7253,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A95" s="19" t="s">
         <v>91</v>
       </c>
@@ -7383,19 +7271,13 @@
       <c r="I95" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J95" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J95" s="14"/>
       <c r="K95" s="14"/>
-      <c r="L95" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L95" s="8"/>
       <c r="M95" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N95" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N95" s="14"/>
       <c r="O95" s="14"/>
       <c r="P95" s="8" t="s">
         <v>359</v>
@@ -7405,9 +7287,7 @@
       <c r="S95" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T95" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T95" s="14"/>
       <c r="U95" s="14"/>
       <c r="V95" s="8" t="s">
         <v>359</v>
@@ -7416,7 +7296,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A96" s="19" t="s">
         <v>97</v>
       </c>
@@ -7434,19 +7314,13 @@
       <c r="I96" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="J96" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="J96" s="14"/>
       <c r="K96" s="14"/>
-      <c r="L96" s="8" t="s">
-        <v>359</v>
-      </c>
+      <c r="L96" s="8"/>
       <c r="M96" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="N96" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="N96" s="14"/>
       <c r="O96" s="14"/>
       <c r="P96" s="8" t="s">
         <v>359</v>
@@ -7456,9 +7330,7 @@
       <c r="S96" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="T96" s="14" t="s">
-        <v>359</v>
-      </c>
+      <c r="T96" s="14"/>
       <c r="U96" s="14"/>
       <c r="V96" s="8" t="s">
         <v>359</v>
@@ -7467,7 +7339,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
         <v>110</v>
       </c>
@@ -7486,7 +7358,7 @@
       <c r="J97" s="14"/>
       <c r="K97" s="14"/>
       <c r="L97" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M97" s="7" t="s">
         <v>359</v>
@@ -7510,7 +7382,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
         <v>99</v>
       </c>
@@ -7531,7 +7403,7 @@
       <c r="J98" s="14"/>
       <c r="K98" s="14"/>
       <c r="L98" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M98" s="7" t="s">
         <v>359</v>
@@ -7555,7 +7427,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
         <v>101</v>
       </c>
@@ -7576,7 +7448,7 @@
       <c r="J99" s="14"/>
       <c r="K99" s="14"/>
       <c r="L99" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M99" s="7" t="s">
         <v>359</v>
@@ -7600,7 +7472,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>302</v>
       </c>
@@ -7621,7 +7493,7 @@
       <c r="J100" s="14"/>
       <c r="K100" s="14"/>
       <c r="L100" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M100" s="7" t="s">
         <v>359</v>
@@ -7649,7 +7521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
         <v>163</v>
       </c>
@@ -7696,7 +7568,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>191</v>
       </c>
@@ -7737,7 +7609,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
         <v>106</v>
       </c>
@@ -7756,7 +7628,7 @@
       <c r="J103" s="14"/>
       <c r="K103" s="14"/>
       <c r="L103" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M103" s="7" t="s">
         <v>359</v>
@@ -7780,7 +7652,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
         <v>363</v>
       </c>
@@ -7821,7 +7693,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
         <v>306</v>
       </c>
@@ -7840,7 +7712,7 @@
       <c r="J105" s="14"/>
       <c r="K105" s="14"/>
       <c r="L105" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M105" s="7" t="s">
         <v>359</v>
@@ -7864,7 +7736,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
         <v>301</v>
       </c>
@@ -7883,7 +7755,7 @@
       <c r="J106" s="14"/>
       <c r="K106" s="14"/>
       <c r="L106" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M106" s="7" t="s">
         <v>359</v>
@@ -7907,9 +7779,9 @@
         <v>339</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="54" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B107" s="55"/>
       <c r="C107" s="56"/>
@@ -7917,11 +7789,11 @@
       <c r="E107" s="56"/>
       <c r="F107" s="56"/>
       <c r="G107" s="57" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H107" s="55"/>
       <c r="I107" s="56" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J107" s="56"/>
       <c r="K107" s="56"/>
@@ -7935,10 +7807,10 @@
         <v>293</v>
       </c>
       <c r="Q107" s="55" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="R107" s="56" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S107" s="56" t="s">
         <v>295</v>
@@ -7950,7 +7822,7 @@
       </c>
       <c r="W107" s="58"/>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
         <v>215</v>
       </c>
@@ -7967,7 +7839,7 @@
       <c r="J108" s="14"/>
       <c r="K108" s="14"/>
       <c r="L108" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M108" s="7" t="s">
         <v>359</v>
@@ -7991,7 +7863,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
         <v>66</v>
       </c>
@@ -8010,7 +7882,7 @@
       <c r="J109" s="14"/>
       <c r="K109" s="14"/>
       <c r="L109" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M109" s="7" t="s">
         <v>359</v>
@@ -8038,7 +7910,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
         <v>55</v>
       </c>
@@ -8057,7 +7929,7 @@
       <c r="J110" s="14"/>
       <c r="K110" s="14"/>
       <c r="L110" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M110" s="7" t="s">
         <v>359</v>
@@ -8085,7 +7957,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
         <v>200</v>
       </c>
@@ -8102,7 +7974,7 @@
       <c r="J111" s="14"/>
       <c r="K111" s="14"/>
       <c r="L111" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M111" s="7" t="s">
         <v>359</v>
@@ -8126,7 +7998,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>217</v>
       </c>
@@ -8143,7 +8015,7 @@
       <c r="J112" s="14"/>
       <c r="K112" s="14"/>
       <c r="L112" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M112" s="7" t="s">
         <v>359</v>
@@ -8167,7 +8039,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
         <v>199</v>
       </c>
@@ -8179,12 +8051,12 @@
       <c r="G113" s="8"/>
       <c r="H113" s="7"/>
       <c r="I113" s="59" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J113" s="14"/>
       <c r="K113" s="14"/>
       <c r="L113" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M113" s="7" t="s">
         <v>359</v>
@@ -8208,7 +8080,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
         <v>319</v>
       </c>
@@ -8225,7 +8097,7 @@
       <c r="J114" s="14"/>
       <c r="K114" s="14"/>
       <c r="L114" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M114" s="7" t="s">
         <v>359</v>
@@ -8249,7 +8121,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
         <v>57</v>
       </c>
@@ -8268,7 +8140,7 @@
       <c r="J115" s="14"/>
       <c r="K115" s="14"/>
       <c r="L115" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M115" s="7" t="s">
         <v>359</v>
@@ -8296,7 +8168,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
         <v>326</v>
       </c>
@@ -8315,7 +8187,7 @@
       <c r="J116" s="14"/>
       <c r="K116" s="14"/>
       <c r="L116" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M116" s="7" t="s">
         <v>359</v>
@@ -8343,7 +8215,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
         <v>370</v>
       </c>
@@ -8362,7 +8234,7 @@
       <c r="J117" s="14"/>
       <c r="K117" s="14"/>
       <c r="L117" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M117" s="7" t="s">
         <v>359</v>
@@ -8386,7 +8258,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
         <v>62</v>
       </c>
@@ -8405,7 +8277,7 @@
       <c r="J118" s="14"/>
       <c r="K118" s="14"/>
       <c r="L118" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M118" s="7" t="s">
         <v>359</v>
@@ -8433,7 +8305,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
         <v>327</v>
       </c>
@@ -8452,7 +8324,7 @@
       <c r="J119" s="14"/>
       <c r="K119" s="14"/>
       <c r="L119" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M119" s="7" t="s">
         <v>359</v>
@@ -8480,7 +8352,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
         <v>206</v>
       </c>
@@ -8497,7 +8369,7 @@
       <c r="J120" s="14"/>
       <c r="K120" s="14"/>
       <c r="L120" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M120" s="7" t="s">
         <v>359</v>
@@ -8521,7 +8393,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
         <v>53</v>
       </c>
@@ -8540,7 +8412,7 @@
       <c r="J121" s="14"/>
       <c r="K121" s="14"/>
       <c r="L121" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M121" s="7" t="s">
         <v>359</v>
@@ -8568,7 +8440,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
         <v>209</v>
       </c>
@@ -8585,7 +8457,7 @@
       <c r="J122" s="14"/>
       <c r="K122" s="14"/>
       <c r="L122" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M122" s="7" t="s">
         <v>359</v>
@@ -8609,7 +8481,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
         <v>197</v>
       </c>
@@ -8626,7 +8498,7 @@
       <c r="J123" s="14"/>
       <c r="K123" s="14"/>
       <c r="L123" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M123" s="7" t="s">
         <v>359</v>
@@ -8650,7 +8522,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
         <v>204</v>
       </c>
@@ -8667,7 +8539,7 @@
       <c r="J124" s="14"/>
       <c r="K124" s="14"/>
       <c r="L124" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M124" s="7" t="s">
         <v>359</v>
@@ -8691,7 +8563,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
         <v>202</v>
       </c>
@@ -8708,7 +8580,7 @@
       <c r="J125" s="14"/>
       <c r="K125" s="14"/>
       <c r="L125" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M125" s="7" t="s">
         <v>359</v>
@@ -8732,7 +8604,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
         <v>51</v>
       </c>
@@ -8751,7 +8623,7 @@
       <c r="J126" s="14"/>
       <c r="K126" s="14"/>
       <c r="L126" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M126" s="7" t="s">
         <v>359</v>
@@ -8779,7 +8651,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
         <v>213</v>
       </c>
@@ -8791,12 +8663,12 @@
       <c r="G127" s="8"/>
       <c r="H127" s="7"/>
       <c r="I127" s="59" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J127" s="14"/>
       <c r="K127" s="14"/>
       <c r="L127" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M127" s="7" t="s">
         <v>359</v>
@@ -8820,7 +8692,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
         <v>342</v>
       </c>
@@ -8839,7 +8711,7 @@
       <c r="J128" s="14"/>
       <c r="K128" s="14"/>
       <c r="L128" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M128" s="7" t="s">
         <v>359</v>
@@ -8867,7 +8739,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
         <v>58</v>
       </c>
@@ -8886,7 +8758,7 @@
       <c r="J129" s="14"/>
       <c r="K129" s="14"/>
       <c r="L129" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M129" s="7" t="s">
         <v>359</v>
@@ -8914,9 +8786,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A130" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B130" s="41"/>
       <c r="C130" s="51"/>
@@ -8955,7 +8827,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A131" s="17" t="s">
         <v>222</v>
       </c>
@@ -8996,7 +8868,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A132" s="17" t="s">
         <v>148</v>
       </c>
@@ -9037,7 +8909,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A133" s="17" t="s">
         <v>321</v>
       </c>
@@ -9078,7 +8950,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A134" s="17" t="s">
         <v>231</v>
       </c>
@@ -9119,7 +8991,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A135" s="17" t="s">
         <v>229</v>
       </c>
@@ -9160,7 +9032,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A136" s="17" t="s">
         <v>233</v>
       </c>
@@ -9201,7 +9073,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A137" s="17" t="s">
         <v>238</v>
       </c>
@@ -9242,7 +9114,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A138" s="17" t="s">
         <v>320</v>
       </c>
@@ -9283,9 +9155,9 @@
         <v>235</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A139" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B139" s="39"/>
       <c r="C139" s="49"/>
@@ -9321,12 +9193,12 @@
         <v>359</v>
       </c>
       <c r="W139" s="60" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="140" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A140" s="18" t="s">
         <v>394</v>
-      </c>
-    </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A140" s="18" t="s">
-        <v>395</v>
       </c>
       <c r="B140" s="41"/>
       <c r="C140" s="51"/>
@@ -9369,7 +9241,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A141" s="19" t="s">
         <v>242</v>
       </c>
@@ -9414,7 +9286,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A142" s="19" t="s">
         <v>224</v>
       </c>
@@ -9459,7 +9331,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A143" s="19" t="s">
         <v>253</v>
       </c>
@@ -9504,7 +9376,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A144" s="19" t="s">
         <v>226</v>
       </c>
@@ -9549,7 +9421,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A145" s="19" t="s">
         <v>251</v>
       </c>
@@ -9594,7 +9466,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A146" s="19" t="s">
         <v>240</v>
       </c>
@@ -9639,7 +9511,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A147" s="19" t="s">
         <v>236</v>
       </c>
@@ -9684,7 +9556,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
         <v>318</v>
       </c>
@@ -9696,12 +9568,12 @@
       <c r="G148" s="8"/>
       <c r="H148" s="7"/>
       <c r="I148" s="59" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J148" s="14"/>
       <c r="K148" s="14"/>
       <c r="L148" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M148" s="7" t="s">
         <v>359</v>
@@ -9725,7 +9597,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A149" s="5" t="s">
         <v>42</v>
       </c>
@@ -9744,7 +9616,7 @@
       <c r="J149" s="14"/>
       <c r="K149" s="14"/>
       <c r="L149" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M149" s="7" t="s">
         <v>359</v>
@@ -9772,7 +9644,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
         <v>247</v>
       </c>
@@ -9789,7 +9661,7 @@
       <c r="J150" s="14"/>
       <c r="K150" s="14"/>
       <c r="L150" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M150" s="7" t="s">
         <v>359</v>
@@ -9813,7 +9685,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A151" s="5" t="s">
         <v>219</v>
       </c>
@@ -9830,7 +9702,7 @@
       <c r="J151" s="14"/>
       <c r="K151" s="14"/>
       <c r="L151" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M151" s="7" t="s">
         <v>359</v>
@@ -9854,7 +9726,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A152" s="5" t="s">
         <v>244</v>
       </c>
@@ -9871,7 +9743,7 @@
       <c r="J152" s="14"/>
       <c r="K152" s="14"/>
       <c r="L152" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M152" s="7" t="s">
         <v>359</v>
@@ -9895,7 +9767,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A153" s="5" t="s">
         <v>245</v>
       </c>
@@ -9912,7 +9784,7 @@
       <c r="J153" s="14"/>
       <c r="K153" s="14"/>
       <c r="L153" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M153" s="7" t="s">
         <v>359</v>
@@ -9936,7 +9808,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A154" s="5" t="s">
         <v>103</v>
       </c>
@@ -9955,7 +9827,7 @@
       <c r="J154" s="14"/>
       <c r="K154" s="14"/>
       <c r="L154" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M154" s="7" t="s">
         <v>359</v>
@@ -9966,10 +9838,10 @@
         <v>359</v>
       </c>
       <c r="Q154" s="27" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="R154" s="59" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="S154" s="14" t="s">
         <v>359</v>
@@ -9983,7 +9855,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A155" s="5" t="s">
         <v>211</v>
       </c>
@@ -9995,12 +9867,12 @@
       <c r="G155" s="8"/>
       <c r="H155" s="7"/>
       <c r="I155" s="59" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J155" s="14"/>
       <c r="K155" s="14"/>
       <c r="L155" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M155" s="7" t="s">
         <v>359</v>
@@ -10024,7 +9896,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A156" s="5" t="s">
         <v>309</v>
       </c>
@@ -10043,7 +9915,7 @@
       <c r="J156" s="14"/>
       <c r="K156" s="14"/>
       <c r="L156" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M156" s="7" t="s">
         <v>359</v>
@@ -10071,7 +9943,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A157" s="5" t="s">
         <v>60</v>
       </c>
@@ -10090,7 +9962,7 @@
       <c r="J157" s="14"/>
       <c r="K157" s="14"/>
       <c r="L157" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M157" s="7" t="s">
         <v>359</v>
@@ -10118,7 +9990,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
         <v>322</v>
       </c>
@@ -10137,7 +10009,7 @@
       <c r="J158" s="14"/>
       <c r="K158" s="14"/>
       <c r="L158" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M158" s="7" t="s">
         <v>359</v>
@@ -10165,7 +10037,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A159" s="5" t="s">
         <v>64</v>
       </c>
@@ -10184,7 +10056,7 @@
       <c r="J159" s="14"/>
       <c r="K159" s="14"/>
       <c r="L159" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M159" s="7" t="s">
         <v>359</v>
@@ -10212,7 +10084,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A160" s="5" t="s">
         <v>49</v>
       </c>
@@ -10231,7 +10103,7 @@
       <c r="J160" s="14"/>
       <c r="K160" s="14"/>
       <c r="L160" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M160" s="7" t="s">
         <v>359</v>
@@ -10259,7 +10131,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A161" s="5" t="s">
         <v>45</v>
       </c>
@@ -10278,7 +10150,7 @@
       <c r="J161" s="14"/>
       <c r="K161" s="14"/>
       <c r="L161" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M161" s="7" t="s">
         <v>359</v>
@@ -10306,7 +10178,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
         <v>47</v>
       </c>
@@ -10325,7 +10197,7 @@
       <c r="J162" s="14"/>
       <c r="K162" s="14"/>
       <c r="L162" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M162" s="7" t="s">
         <v>359</v>
@@ -10353,7 +10225,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A163" s="61" t="s">
         <v>300</v>
       </c>
@@ -10380,7 +10252,7 @@
       <c r="V163" s="64"/>
       <c r="W163" s="65"/>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A164" s="21" t="s">
         <v>166</v>
       </c>
@@ -10421,7 +10293,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A165" s="21" t="s">
         <v>172</v>
       </c>
@@ -10462,7 +10334,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A166" s="21" t="s">
         <v>348</v>
       </c>
@@ -10531,7 +10403,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A167" s="21" t="s">
         <v>140</v>
       </c>
@@ -10572,7 +10444,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A168" s="5" t="s">
         <v>274</v>
       </c>
@@ -10587,7 +10459,7 @@
       <c r="J168" s="14"/>
       <c r="K168" s="14"/>
       <c r="L168" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M168" s="7"/>
       <c r="N168" s="14"/>
@@ -10609,7 +10481,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A169" s="5" t="s">
         <v>349</v>
       </c>
@@ -10624,7 +10496,7 @@
       <c r="J169" s="14"/>
       <c r="K169" s="14"/>
       <c r="L169" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M169" s="7" t="s">
         <v>359</v>
@@ -10644,7 +10516,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A170" s="5" t="s">
         <v>350</v>
       </c>
@@ -10659,7 +10531,7 @@
       <c r="J170" s="14"/>
       <c r="K170" s="14"/>
       <c r="L170" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M170" s="7" t="s">
         <v>359</v>
@@ -10683,7 +10555,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A171" s="21" t="s">
         <v>176</v>
       </c>
@@ -10724,7 +10596,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A172" s="5" t="s">
         <v>265</v>
       </c>
@@ -10739,7 +10611,7 @@
       <c r="J172" s="14"/>
       <c r="K172" s="14"/>
       <c r="L172" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M172" s="7"/>
       <c r="N172" s="14"/>
@@ -10761,7 +10633,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A173" s="21" t="s">
         <v>153</v>
       </c>

</xml_diff>